<commit_message>
Update data/fitur terbaru dari VPS
</commit_message>
<xml_diff>
--- a/back/public/dealer/files/salesorder/excel/salesorder_33.xlsx
+++ b/back/public/dealer/files/salesorder/excel/salesorder_33.xlsx
@@ -26,13 +26,13 @@
     <t>SOLD TO:</t>
   </si>
   <si>
-    <t>CV Maju Abadi - jakartaa</t>
+    <t>Gala Jaya - Pontianak - Sulawesi</t>
   </si>
   <si>
     <t>SO NO</t>
   </si>
   <si>
-    <t>SS-01/101/19/JUL/2025</t>
+    <t>SS-10/#8003/21/JUL/2025</t>
   </si>
   <si>
     <t>DELIVERED TO:</t>
@@ -44,7 +44,7 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>7/15/2025</t>
+    <t>7/21/2025</t>
   </si>
   <si>
     <t>PHONE:</t>
@@ -119,7 +119,7 @@
     <t>SALES PERSONNEL</t>
   </si>
   <si>
-    <t>alfredo dagonza</t>
+    <t>superadminnn</t>
   </si>
 </sst>
 </file>
@@ -747,7 +747,7 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
@@ -913,7 +913,7 @@
         <v>26</v>
       </c>
       <c r="D16" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>27</v>
@@ -922,13 +922,13 @@
         <v>30000</v>
       </c>
       <c r="G16" s="10">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="H16" s="10">
-        <v>60000</v>
+        <v>33300</v>
       </c>
       <c r="I16" s="10">
-        <v>120000</v>
+        <v>33300</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -943,7 +943,7 @@
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="12">
-        <v>120000</v>
+        <v>33300</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>